<commit_message>
시럼 끝! - 50_6의 unknown 비율에 따른 instance 및 sequence 실험 (table 2) - 50의 unknown 비율이 10% 및 20% 일 때 instance 실험 - 50의 unknown 비율이 10% 및 20% 일 때 sequence 실험 (Table 3) - 50의 unknown 비율에 따른 instance 및 sequence 실험 (table 2) - 그리고 위 실험 결과를 위한 실험 데이터
</commit_message>
<xml_diff>
--- a/result161101.xlsx
+++ b/result161101.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="50_6(FREQ,PW,dTOA)" sheetId="1" r:id="rId1"/>
+    <sheet name="50(FREQ,PW,dTOA)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>dsa</t>
   </si>
@@ -55,6 +56,26 @@
   </si>
   <si>
     <t>50개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown 비율이 10%일 때 instance 실험
+(논문에 기제된 표 번호: 없음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown 비율이 20%일 때 instance 실험
+(논문에 기제된 표 번호: 없음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown 비율이 20%일 때 instance 실험
+(논문에 기제된 표 번호: Table 3-b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown 비율이 10%일 때 instance 실험
+(논문에 기제된 표 번호: Table 3-a)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +125,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -113,6 +134,12 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -394,14 +421,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L22"/>
+  <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>0.1</v>
@@ -594,6 +637,22 @@
         <v>0.94619602008023429</v>
       </c>
     </row>
+    <row r="8" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>0.1</v>
@@ -785,6 +844,18 @@
       <c r="L14">
         <v>0.97542462464175195</v>
       </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -910,6 +981,27 @@
   <sortState ref="H10:L14">
     <sortCondition ref="H10"/>
   </sortState>
+  <mergeCells count="6">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="H16:L16"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>